<commit_message>
Update EX-HX-Combo jumper planning document.
</commit_message>
<xml_diff>
--- a/EX-HX-Combo/Jumper Planning.xlsx
+++ b/EX-HX-Combo/Jumper Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ISA-Cards\EX-HX-Combo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28D517A-4731-4BBA-8233-45C040A7D9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9322D0-BED6-47AC-9198-36803534A5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" activeTab="1" xr2:uid="{53E6B26A-4FC4-4028-AFDD-E83FA1776CB0}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="67">
   <si>
     <t>Jumper(s)</t>
   </si>
@@ -198,6 +198,36 @@
   </si>
   <si>
     <t>D000/UMB 96K</t>
+  </si>
+  <si>
+    <t>1100 1</t>
+  </si>
+  <si>
+    <t>1110 1</t>
+  </si>
+  <si>
+    <t>1101 0</t>
+  </si>
+  <si>
+    <t>1101 1</t>
+  </si>
+  <si>
+    <t>1110 0</t>
+  </si>
+  <si>
+    <t>0110 0</t>
+  </si>
+  <si>
+    <t>0000 1</t>
+  </si>
+  <si>
+    <t>0110 1</t>
+  </si>
+  <si>
+    <t>0111 0</t>
+  </si>
+  <si>
+    <t>0111 1</t>
   </si>
 </sst>
 </file>
@@ -213,7 +243,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +286,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6FAF4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -293,7 +329,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -304,17 +340,23 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF6FAF4"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -651,14 +693,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>6</v>
       </c>
     </row>
@@ -750,10 +792,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22E4EACD-87F3-485F-ACBC-743F19FFEC29}">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,12 +804,13 @@
     <col min="2" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>27</v>
       </c>
@@ -789,46 +832,49 @@
       <c r="G1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>56</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>32</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
       <c r="B3" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
       <c r="B5" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="5">
@@ -841,8 +887,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -853,8 +899,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="5">
@@ -867,8 +913,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
       <c r="B9" s="5">
         <v>7</v>
       </c>
@@ -879,8 +925,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="6">
@@ -891,8 +937,8 @@
       </c>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
       <c r="B11" s="6">
         <v>9</v>
       </c>
@@ -901,8 +947,8 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="6">
@@ -913,8 +959,8 @@
       </c>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
       <c r="B13" s="6">
         <v>11</v>
       </c>
@@ -923,71 +969,92 @@
       </c>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="8"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="8"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="B14" s="13">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13">
+        <v>13</v>
+      </c>
+      <c r="H15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="8"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="8"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="B16" s="13">
+        <v>14</v>
+      </c>
+      <c r="H16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="J26" s="4">
+      <c r="H26" s="8"/>
+      <c r="K26" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
       <c r="E27" s="7">
         <v>13</v>
       </c>
@@ -997,15 +1064,18 @@
       <c r="G27" s="7">
         <v>13</v>
       </c>
-      <c r="I27" s="4">
-        <v>1</v>
+      <c r="H27" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="J27" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="K27" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="7">
@@ -1017,12 +1087,15 @@
       <c r="G28" s="7">
         <v>14</v>
       </c>
-      <c r="H28" s="9"/>
+      <c r="H28" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
+      <c r="K28" s="9"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
       <c r="E29" s="7">
         <v>15</v>
       </c>
@@ -1032,8 +1105,8 @@
       <c r="G29" s="7">
         <v>15</v>
       </c>
-      <c r="H29" s="7">
-        <v>13</v>
+      <c r="H29" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="I29" s="7">
         <v>13</v>
@@ -1041,9 +1114,12 @@
       <c r="J29" s="7">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="K29" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
         <v>25</v>
       </c>
       <c r="F30" s="7">
@@ -1052,8 +1128,8 @@
       <c r="G30" s="7">
         <v>12</v>
       </c>
-      <c r="H30" s="7">
-        <v>14</v>
+      <c r="H30" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="I30" s="7">
         <v>14</v>
@@ -1061,14 +1137,17 @@
       <c r="J30" s="7">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
+      <c r="K30" s="7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
       <c r="G31" s="4">
         <v>1</v>
       </c>
-      <c r="H31" s="7">
-        <v>15</v>
+      <c r="H31" s="8" t="s">
+        <v>58</v>
       </c>
       <c r="I31" s="7">
         <v>15</v>
@@ -1076,14 +1155,17 @@
       <c r="J31" s="7">
         <v>15</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="K31" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
+      <c r="A33" s="12"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
@@ -1174,11 +1256,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
@@ -1190,6 +1267,11 @@
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1209,13 +1291,13 @@
       <c r="A1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>39</v>
       </c>
       <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="11">
+      <c r="D1" s="10">
         <v>0</v>
       </c>
     </row>
@@ -1223,13 +1305,13 @@
       <c r="A2" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="10">
         <v>0</v>
       </c>
     </row>
@@ -1237,18 +1319,18 @@
       <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="10">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>42</v>
       </c>
       <c r="C6" t="s">

</xml_diff>